<commit_message>
Improved templates and changes to the data set for rendering
</commit_message>
<xml_diff>
--- a/data/IT-куб.xlsx
+++ b/data/IT-куб.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>patronymic</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Визуальное программирование</t>
+  </si>
+  <si>
+    <t>без модуля</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -620,7 +623,7 @@
         <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3">
         <v>136</v>
@@ -646,13 +649,13 @@
         <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3">
         <v>136</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>20</v>
@@ -672,7 +675,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3">
         <v>136</v>
@@ -697,15 +700,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>cert_data!$B$1:$B$3</xm:f>
+            <xm:f>cert_data!$C$1:$C$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E4</xm:sqref>
+          <xm:sqref>D2:D4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>cert_data!$C$1:$C$14</xm:f>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D4</xm:sqref>
+          <xm:sqref>E2:E4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -718,7 +721,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -759,6 +762,9 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
The design of the text for the console was added and a build of the program was made.
</commit_message>
<xml_diff>
--- a/data/IT-куб.xlsx
+++ b/data/IT-куб.xlsx
@@ -9,11 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Python" sheetId="7" r:id="rId1"/>
-    <sheet name="cert_data" sheetId="9" r:id="rId2"/>
+    <sheet name="Кибергигиена" sheetId="16" r:id="rId1"/>
+    <sheet name="Python" sheetId="7" r:id="rId2"/>
+    <sheet name="VRAR" sheetId="11" r:id="rId3"/>
+    <sheet name="ОАЛ" sheetId="15" r:id="rId4"/>
+    <sheet name="МР" sheetId="13" r:id="rId5"/>
+    <sheet name="ОК" sheetId="17" r:id="rId6"/>
+    <sheet name="ПР" sheetId="12" r:id="rId7"/>
+    <sheet name="СА" sheetId="14" r:id="rId8"/>
+    <sheet name="СП" sheetId="18" r:id="rId9"/>
+    <sheet name="cert_data" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="29">
   <si>
     <t>patronymic</t>
   </si>
@@ -45,24 +53,9 @@
     <t>Программирование роботов</t>
   </si>
   <si>
-    <t>Владимирович</t>
-  </si>
-  <si>
-    <t>Владимир</t>
-  </si>
-  <si>
     <t>углубленный модуль</t>
   </si>
   <si>
-    <t>Ольга</t>
-  </si>
-  <si>
-    <t>Александровна</t>
-  </si>
-  <si>
-    <t>Вероника</t>
-  </si>
-  <si>
     <t>Кибергигиена и работа с большими данными</t>
   </si>
   <si>
@@ -78,24 +71,6 @@
     <t>Основы алгоритмики и логики</t>
   </si>
   <si>
-    <t>Кулешова</t>
-  </si>
-  <si>
-    <t>Вышеславцев</t>
-  </si>
-  <si>
-    <t>№2024/0355</t>
-  </si>
-  <si>
-    <t>№2024/0356</t>
-  </si>
-  <si>
-    <t>Кравцова</t>
-  </si>
-  <si>
-    <t>№2024/0363</t>
-  </si>
-  <si>
     <t>course</t>
   </si>
   <si>
@@ -142,13 +117,16 @@
   </si>
   <si>
     <t>без модуля</t>
+  </si>
+  <si>
+    <t>Мобильная разработка</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +153,13 @@
       <b/>
       <sz val="16"/>
       <color rgb="FF1F2328"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1A1A1A"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -221,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -239,17 +224,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,10 +554,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="40.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Iz9XpwAHqxcpehazFnKokvtbK9GrewYjTCHG0Po8jGjFw+ZgyH0jod5ZWUC0wBJCJ+SfOCgoS+ZUkfrX3izONA==" saltValue="P8CN7ocJ138vUTRXYJNEbg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sortState ref="C11:C15">
+    <sortCondition ref="C11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -583,109 +805,47 @@
     <col min="8" max="8" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="3">
-        <v>136</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3">
-        <v>136</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3">
-        <v>136</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="H2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -696,19 +856,19 @@
           <x14:formula1>
             <xm:f>cert_data!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>cert_data!$C$1:$C$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D4</xm:sqref>
+          <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>cert_data!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E4</xm:sqref>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -716,110 +876,639 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="28.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C6" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C7" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C8" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C10" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C11" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C12" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C13" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C14" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="H2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="27.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$B$1:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>cert_data!$C$1:$C$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>